<commit_message>
Lots of work done
</commit_message>
<xml_diff>
--- a/data/providers1.xlsx
+++ b/data/providers1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>Adults</t>
   </si>
@@ -58,16 +58,28 @@
     <t>http://www.cmsj.org/chinmaya-bala-vihar/location/fremont/</t>
   </si>
   <si>
+    <t>wwe2</t>
+  </si>
+  <si>
     <t>Tamil</t>
   </si>
   <si>
-    <t>Newtab</t>
-  </si>
-  <si>
     <t>dff</t>
   </si>
   <si>
     <t>IIT Delhi</t>
+  </si>
+  <si>
+    <t>mohit.com</t>
+  </si>
+  <si>
+    <t>Pets</t>
+  </si>
+  <si>
+    <t>s333</t>
+  </si>
+  <si>
+    <t>sdse3</t>
   </si>
 </sst>
 </file>
@@ -75,53 +87,53 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="7">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
       <sz val="10"/>
-    </font>
-    <font>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
       <sz val="10"/>
-    </font>
-    <font>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="9"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="9"/>
-    </font>
-    <font>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF0563C1"/>
-      <sz val="9"/>
-      <u val="single"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF0563C1"/>
-      <sz val="11"/>
-      <u val="single"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,14 +145,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thick"/>
       <right style="thick"/>
       <top style="thick"/>
@@ -149,68 +161,72 @@
     </border>
   </borders>
   <cellStyleXfs count="21">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="6" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="20">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+  <cellXfs count="7">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -282,8 +298,8 @@
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C5" activeCellId="0" pane="topLeft" sqref="C5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -298,7 +314,7 @@
     <col collapsed="false" hidden="false" max="1025" min="8" style="2" width="9.1417004048583"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="11.9" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="11.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -320,8 +336,10 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="32.8" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -346,15 +364,15 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="32.8" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="n">
-        <v>23333</v>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>9</v>
@@ -369,113 +387,117 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="0" t="s">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="0"/>
+      <c r="G4" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="D5" s="0" t="s">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="0"/>
+      <c r="G5" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="22"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="24"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="25"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="28"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="29"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="30"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="31"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="32"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="33"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="34"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="35"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="36"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="37"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="38"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="39"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="40"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="41"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="42"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="43"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="44"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="45"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="46"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="47"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="48"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="49"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="50"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="51"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="52"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="53"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="54"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="55"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="56"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="57"/>
+    <row r="6" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="http://www.annapoklewskiacademyofmusic.com/" ref="G1" r:id="rId1"/>
-    <hyperlink display="http://www.cmsj.org/chinmaya-bala-vihar/location/fremont/" ref="G2" r:id="rId2"/>
-    <hyperlink display="http://www.cmsj.org/chinmaya-bala-vihar/location/fremont/" ref="G3" r:id="rId3"/>
+    <hyperlink ref="G1" r:id="rId1" display="http://www.annapoklewskiacademyofmusic.com/"/>
+    <hyperlink ref="G2" r:id="rId2" display="http://www.cmsj.org/chinmaya-bala-vihar/location/fremont/"/>
+    <hyperlink ref="G3" r:id="rId3" display="http://www.cmsj.org/chinmaya-bala-vihar/location/fremont/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>